<commit_message>
adding functionality of export button disabled
</commit_message>
<xml_diff>
--- a/electron/YouTube_API_Test/1-TestFile.xlsx
+++ b/electron/YouTube_API_Test/1-TestFile.xlsx
@@ -4,10 +4,60 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>FREECODE</t>
+  </si>
+  <si>
+    <t>10-06-2020</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9sWEecNUW-o</t>
+  </si>
+  <si>
+    <t>Code your own YouTube app: YouTube API + HTML + CSS + JavaScript (full tutorial)</t>
+  </si>
+  <si>
+    <t>1-TestFile</t>
+  </si>
+  <si>
+    <t>PT1H7M35S</t>
+  </si>
+  <si>
+    <t>freeCodeCamp.org</t>
+  </si>
+  <si>
+    <t>2060000</t>
+  </si>
+  <si>
+    <t>2014-12-16T21:18:48Z</t>
+  </si>
+  <si>
+    <t>1114</t>
+  </si>
+  <si>
+    <t>74760</t>
+  </si>
+  <si>
+    <t>1297</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,7 +435,53 @@
   <dimension ref="C1:AY1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="3:51" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>